<commit_message>
adding revisions to folder structure
</commit_message>
<xml_diff>
--- a/datasetsNotes.xlsx
+++ b/datasetsNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/christie_barron_mail_utoronto_ca/Documents/bootcamp/AITextDetector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5593F501-5F1A-5141-8226-A21E4B61B548}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4046CE0E-5334-7744-8EB0-6DFFA385E483}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1980" windowWidth="25600" windowHeight="19980" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Dataset Name</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yash's (TA) feedback on my question about our data: 1) focused on problem/concept first. 2) more data, better accuracy (features and sample size). 3) web scraping is an advanced thing so its more difficult. Is a good challenge and will look good, but is not compulsatory and is advanced/challenging. . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">STARTING WITH THIS DATASET. </t>
   </si>
 </sst>
 </file>
@@ -248,6 +251,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,12 +557,12 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="47.1640625" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="1" customWidth="1"/>
     <col min="3" max="4" width="36.33203125" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" customWidth="1"/>
@@ -585,6 +592,9 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
       <c r="E2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
adding additional data and template code
</commit_message>
<xml_diff>
--- a/datasetsNotes.xlsx
+++ b/datasetsNotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/christie_barron_mail_utoronto_ca/Documents/bootcamp/AITextDetector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4046CE0E-5334-7744-8EB0-6DFFA385E483}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{B1F0CA58-295A-C24D-BC8A-FCDF101539AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2B10073-A359-6245-8F07-FB0B2CBCA12E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{14DD702A-460B-8E49-9953-BD9819A77AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,7 +186,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,6 +199,14 @@
       <color rgb="FF123654"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -224,10 +232,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -236,8 +245,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -557,7 +568,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -624,7 +635,7 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="1"/>
@@ -763,6 +774,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{FE61863E-14EA-3548-839B-01AFF8A88E98}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>